<commit_message>
fixed class names on excel files
</commit_message>
<xml_diff>
--- a/docs/unit1/02_head/Excel files/cylinder.xlsx
+++ b/docs/unit1/02_head/Excel files/cylinder.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Documents\Courses\CE 544\in-class tasks\1. hyrdraulic head\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/ce547/docs/unit1/02_head/Excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CC4645-9E73-1D4C-8B64-AEDFFB85FD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27090" windowHeight="13185"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27100" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,13 +30,13 @@
     <t>Head Calculations</t>
   </si>
   <si>
-    <t>CE En 544 - Brigham Young University</t>
+    <t>CE 544 - Brigham Young University</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,7 +126,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -184,15 +191,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>276225</xdr:colOff>
+          <xdr:colOff>279400</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>295275</xdr:colOff>
+          <xdr:colOff>292100</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>88900</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -200,6 +207,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -214,32 +224,21 @@
               <a:avLst/>
             </a:prstGeom>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+              <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
             <a:extLst>
               <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
                 <a14:hiddenLine w="9525">
                   <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                    <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:prstDash val="solid"/>
                   <a:miter lim="800000"/>
                   <a:headEnd/>
-                  <a:tailEnd type="none" w="med" len="med"/>
+                  <a:tailEnd/>
                 </a14:hiddenLine>
-              </a:ext>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
               </a:ext>
             </a:extLst>
           </xdr:spPr>
@@ -514,60 +513,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
     </row>
   </sheetData>
@@ -582,15 +581,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
+                <xdr:colOff>279400</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
+                <xdr:colOff>292100</xdr:colOff>
                 <xdr:row>16</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:rowOff>88900</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>